<commit_message>
增加对currentUser变量的获取和判断，否则会报500 (Internal server error)
</commit_message>
<xml_diff>
--- a/表结构.xlsx
+++ b/表结构.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>标题</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -95,6 +95,34 @@
   </si>
   <si>
     <t>用户ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Post</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>title</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attachment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>remarks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>records</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -154,10 +182,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -452,129 +480,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="14.25" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9">
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="C1" s="1"/>
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1" t="s">
+    <row r="2" spans="1:9">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="E4" s="1" t="s">
+      <c r="C4" s="1"/>
+      <c r="F4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="E5" s="1" t="s">
+      <c r="C5" s="1"/>
+      <c r="F5" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="1" t="s">
+      <c r="H5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="E6" s="1" t="s">
+      <c r="C6" s="1"/>
+      <c r="F6" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="1" t="s">
+      <c r="H6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:9">
+      <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="2"/>
-      <c r="B9" s="1" t="s">
+    <row r="9" spans="1:9">
+      <c r="B9" s="3"/>
+      <c r="C9" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="2"/>
-      <c r="B10" s="1" t="s">
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="2"/>
-      <c r="B11" s="1" t="s">
+    <row r="11" spans="1:9">
+      <c r="B11" s="3"/>
+      <c r="C11" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="2"/>
-      <c r="B12" s="1" t="s">
+    <row r="12" spans="1:9">
+      <c r="B12" s="3"/>
+      <c r="C12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="3"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="B8:B12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>